<commit_message>
BD local e Mock
</commit_message>
<xml_diff>
--- a/arquitetura/Arquitetura do Software.xlsx
+++ b/arquitetura/Arquitetura do Software.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rnappi\Documents\GitHub\tcc-app\arquitetura\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\tcc-app\arquitetura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ABBC7B5-5E5C-4EA9-A283-9D7E55BC6C9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F5ABF69-C010-419D-A6A1-F8ADF72B5A9A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -73,9 +73,6 @@
     <t>Cria uma nova tentativa</t>
   </si>
   <si>
-    <t>/api/alunos/{id_aluno}/tentativas/?questionarios={id_questionario}</t>
-  </si>
-  <si>
     <t>Lista as tentativas do aluno podendo filtrar por questionarios</t>
   </si>
   <si>
@@ -95,6 +92,9 @@
   </si>
   <si>
     <t>/api/tentativas</t>
+  </si>
+  <si>
+    <t>/api/alunos/{id_aluno}/tentativas/questionario/{id_questionario}</t>
   </si>
 </sst>
 </file>
@@ -1068,8 +1068,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:D25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1107,13 +1107,13 @@
     </row>
     <row r="18" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1151,13 +1151,13 @@
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
@@ -1168,12 +1168,12 @@
         <v>3</v>
       </c>
       <c r="D23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>4</v>
@@ -1184,13 +1184,13 @@
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>